<commit_message>
DatDF now has two level index and passes unittests
</commit_message>
<xml_diff>
--- a/tests/fixtures/DataFrames/new.xlsx
+++ b/tests/fixtures/DataFrames/new.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:D1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -367,9 +367,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>datnum</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>datnum</t>
+          <t>datname</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -380,6 +385,44 @@
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>picklepath</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>x_label</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>y_label</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>base</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1577779312.350123</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>pathtopickle</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>xlabel</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>ylabel</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Made way to add/edit column indexes easily
</commit_message>
<xml_diff>
--- a/tests/fixtures/DataFrames/new.xlsx
+++ b/tests/fixtures/DataFrames/new.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -397,6 +397,16 @@
           <t>y_label</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>dim</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>time_elapsed</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -407,8 +417,10 @@
           <t>base</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>1577779312.350123</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Wednesday, January 1, 2020 00:00:00</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -424,6 +436,12 @@
         <is>
           <t>ylabel</t>
         </is>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>